<commit_message>
Warnings varios y errores en spawn flame corregidos, trayectoria de moneda parabólica, transición de nivel mejorada
</commit_message>
<xml_diff>
--- a/Bug report.xlsx
+++ b/Bug report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Bug #</t>
   </si>
@@ -97,6 +97,42 @@
   </si>
   <si>
     <t>Resuelto en branch bugs1</t>
+  </si>
+  <si>
+    <t>El león debe tener hitbox de las patas delanteras para no caer debajo de la línea del suelo</t>
+  </si>
+  <si>
+    <t>El puntaje se resetea al pasar de nivel</t>
+  </si>
+  <si>
+    <t>Habrá que usar la misma instancia del HUD en todos los niveles o tener el puntaje en global?</t>
+  </si>
+  <si>
+    <t>Falta sonido al sumar el timer al puntaje al final del nivel</t>
+  </si>
+  <si>
+    <t>El sonido a usar es Circus Charlie SFX (6)</t>
+  </si>
+  <si>
+    <t>Contemplar caso que el puntaje se termine de sumar antes de que termine la música al ganar el nivel</t>
+  </si>
+  <si>
+    <t>Esperar 2 condiciones: que termine la música y que termine de sumar el puntaje</t>
+  </si>
+  <si>
+    <t>Posiblemente resuelto</t>
+  </si>
+  <si>
+    <t>El león no se alinea al final si queda descentrado en la plataforma</t>
+  </si>
+  <si>
+    <t>Si no queda centrado al ganar, mover lentamente hacia el centro de la plataforma</t>
+  </si>
+  <si>
+    <t>En la animación de Charlie al correr, los pies deberían mantenerse en la misma posición y moverse el cuerpo, ahora se mueven los pies y el cuerpo queda en la misma posición</t>
+  </si>
+  <si>
+    <t>Corregir el sprite en un pixel para que no se de ese efecto</t>
   </si>
 </sst>
 </file>
@@ -169,8 +205,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -580,13 +636,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -660,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>6</v>
@@ -730,6 +786,9 @@
       <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="30">
       <c r="A9" s="3">
@@ -753,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>18</v>
@@ -813,7 +872,114 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:6" ht="30">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:F1048576">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$C1="Resuelto"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$C1="Abierto"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>